<commit_message>
Changed Hirose Prefix, added Honeywell MPRL series transducer, updated manufacturer prefix table
- Changed HIROSE prefix to HRS
- Updated component manufacturer prefixes table
- Added Honeywell MPR long port gage and no gage models
- Added HW_MPR_Long-Port footprints
- Added HW_MPRLS0025PA00001A symbol
</commit_message>
<xml_diff>
--- a/Reference Documents/Component Manufacturer Prefixes.xlsx
+++ b/Reference Documents/Component Manufacturer Prefixes.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$C$37</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$C$39</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -36,6 +36,18 @@
     <t>ADESTO</t>
   </si>
   <si>
+    <t>Allegro Microsystems</t>
+  </si>
+  <si>
+    <t>ALLEGRO</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
     <t>Analog Devices</t>
   </si>
   <si>
@@ -45,18 +57,6 @@
     <t>Companies purchased by AD retain original prefixes</t>
   </si>
   <si>
-    <t>Allegro Microsystems</t>
-  </si>
-  <si>
-    <t>ALLEGRO</t>
-  </si>
-  <si>
-    <t>Amphenol</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
     <t>BIVAR</t>
   </si>
   <si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>HARWIN</t>
+  </si>
+  <si>
+    <t>Hirose</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>Honeywell</t>
+  </si>
+  <si>
+    <t>HW</t>
   </si>
   <si>
     <t>Integrated Silicon Solutions, Inc</t>
@@ -575,27 +587,27 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
@@ -694,7 +706,7 @@
       <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -703,7 +715,7 @@
       <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
@@ -721,27 +733,27 @@
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="C20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="7"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
@@ -775,22 +787,22 @@
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="6"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>56</v>
@@ -878,8 +890,30 @@
       </c>
       <c r="C37" s="6"/>
     </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$C$37"/>
+  <autoFilter ref="$A$1:$C$39">
+    <sortState ref="A1:C39">
+      <sortCondition ref="A1:A39"/>
+    </sortState>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>